<commit_message>
add reptilia i.e., avians to species as a tab in excel file
</commit_message>
<xml_diff>
--- a/data/species.xlsx
+++ b/data/species.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vanderbilt365-my.sharepoint.com/personal/linhe_xu_vanderbilt_edu/Documents/Herculano_Lab/2020_dNdS_paper/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vanderbilt365-my.sharepoint.com/personal/linhe_xu_vanderbilt_edu/Documents/Herculano_Lab/Projects/neuron-glia-dNdS/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{4A072DEC-4193-E94B-9964-BF2BE1F54BE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{318CEDD6-B596-194F-8DF4-3B2F3494FBF6}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{4A072DEC-4193-E94B-9964-BF2BE1F54BE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5DCD15EE-456F-8B4E-95B1-084FC1E0BBF4}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15660" xr2:uid="{AEE5C36A-4567-E24F-876A-9B3B980CB6BB}"/>
+    <workbookView xWindow="-29320" yWindow="-920" windowWidth="28800" windowHeight="15660" xr2:uid="{AEE5C36A-4567-E24F-876A-9B3B980CB6BB}"/>
   </bookViews>
   <sheets>
-    <sheet name="List of Species" sheetId="4" r:id="rId1"/>
+    <sheet name="Mammals" sheetId="4" r:id="rId1"/>
+    <sheet name="Reptilia" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="407">
   <si>
     <t>Algerian mouse</t>
   </si>
@@ -585,9 +586,6 @@
     <t>Mus spretus</t>
   </si>
   <si>
-    <t xml:space="preserve">Colobus angloensis </t>
-  </si>
-  <si>
     <t>Dasypus novemcinctus</t>
   </si>
   <si>
@@ -729,12 +727,6 @@
     <t>Didelphimorphia</t>
   </si>
   <si>
-    <t xml:space="preserve">Pongo abelii </t>
-  </si>
-  <si>
-    <t>Aliuropoda melanoleuca</t>
-  </si>
-  <si>
     <t>Sus scrofa</t>
   </si>
   <si>
@@ -916,6 +908,345 @@
   </si>
   <si>
     <t>Mus musculus</t>
+  </si>
+  <si>
+    <t>Abingdon island giant tortoise</t>
+  </si>
+  <si>
+    <t>cabingdonii</t>
+  </si>
+  <si>
+    <t>Agassiz's desert tortoise</t>
+  </si>
+  <si>
+    <t>gagassizii</t>
+  </si>
+  <si>
+    <t>Argentine black and white tegu</t>
+  </si>
+  <si>
+    <t>smerianae</t>
+  </si>
+  <si>
+    <t>Anole lizard</t>
+  </si>
+  <si>
+    <t>acarolinensis</t>
+  </si>
+  <si>
+    <t>Australian saltwater crocodile</t>
+  </si>
+  <si>
+    <t>cporosus</t>
+  </si>
+  <si>
+    <t>Bengalese finch</t>
+  </si>
+  <si>
+    <t>lsdomestica</t>
+  </si>
+  <si>
+    <t>Blue tit</t>
+  </si>
+  <si>
+    <t>ccaeruleus</t>
+  </si>
+  <si>
+    <t>Blue-crowned manakin</t>
+  </si>
+  <si>
+    <t>lcoronata</t>
+  </si>
+  <si>
+    <t>Budgerigar</t>
+  </si>
+  <si>
+    <t>mundulatus</t>
+  </si>
+  <si>
+    <t>Chilean tinamou</t>
+  </si>
+  <si>
+    <t>nperdicaria</t>
+  </si>
+  <si>
+    <t>Chinese softshell turtle</t>
+  </si>
+  <si>
+    <t>psinensis</t>
+  </si>
+  <si>
+    <t>Common canary</t>
+  </si>
+  <si>
+    <t>scanaria</t>
+  </si>
+  <si>
+    <t>Dark-eyed junco</t>
+  </si>
+  <si>
+    <t>jhyemalis</t>
+  </si>
+  <si>
+    <t>Duck</t>
+  </si>
+  <si>
+    <t>applatyrhynchos</t>
+  </si>
+  <si>
+    <t>Emu</t>
+  </si>
+  <si>
+    <t>dnovaehollandiae</t>
+  </si>
+  <si>
+    <t>Flycatcher</t>
+  </si>
+  <si>
+    <t>falbicollis</t>
+  </si>
+  <si>
+    <t>Golden-collared manakin</t>
+  </si>
+  <si>
+    <t>mvitellinus</t>
+  </si>
+  <si>
+    <t>Great Tit</t>
+  </si>
+  <si>
+    <t>pmajor</t>
+  </si>
+  <si>
+    <t>Great spotted kiwi</t>
+  </si>
+  <si>
+    <t>ahaastii</t>
+  </si>
+  <si>
+    <t>Helmeted guineafowl</t>
+  </si>
+  <si>
+    <t>nmeleagris</t>
+  </si>
+  <si>
+    <t>Japanese quail</t>
+  </si>
+  <si>
+    <t>cjaponica</t>
+  </si>
+  <si>
+    <t>Little spotted kiwi</t>
+  </si>
+  <si>
+    <t>aowenii</t>
+  </si>
+  <si>
+    <t>Okarito brown kiwi</t>
+  </si>
+  <si>
+    <t>arowi</t>
+  </si>
+  <si>
+    <t>Painted turtle</t>
+  </si>
+  <si>
+    <t>cpbellii</t>
+  </si>
+  <si>
+    <t>Pink-footed goose</t>
+  </si>
+  <si>
+    <t>abrachyrhynchus</t>
+  </si>
+  <si>
+    <t>Ruff</t>
+  </si>
+  <si>
+    <t>cpugnax</t>
+  </si>
+  <si>
+    <t>Spoon-billed sandpiper</t>
+  </si>
+  <si>
+    <t>cpygmaea</t>
+  </si>
+  <si>
+    <t>Tuatara</t>
+  </si>
+  <si>
+    <t>spunctatus</t>
+  </si>
+  <si>
+    <t>Turkey</t>
+  </si>
+  <si>
+    <t>mgallopavo</t>
+  </si>
+  <si>
+    <t>White-throated sparrow</t>
+  </si>
+  <si>
+    <t>zalbicollis</t>
+  </si>
+  <si>
+    <t>Zebra Finch</t>
+  </si>
+  <si>
+    <t>tguttata</t>
+  </si>
+  <si>
+    <t>Chelonoidis abingdonii</t>
+  </si>
+  <si>
+    <t>Gopherus agassizii</t>
+  </si>
+  <si>
+    <t>Anolis carolinensis</t>
+  </si>
+  <si>
+    <t>Salvator merianae</t>
+  </si>
+  <si>
+    <t>Crocodylus porosus</t>
+  </si>
+  <si>
+    <t>Lonchura striata domestica</t>
+  </si>
+  <si>
+    <t>Cyanistes caeruleus</t>
+  </si>
+  <si>
+    <t>Lepidothrix coronata</t>
+  </si>
+  <si>
+    <t>Melopsittacus undulatus</t>
+  </si>
+  <si>
+    <t>Nothoprocta perdicaria</t>
+  </si>
+  <si>
+    <t>Pelodiscus sinensis</t>
+  </si>
+  <si>
+    <t>Serinus canaria</t>
+  </si>
+  <si>
+    <t>Junco hyemalis</t>
+  </si>
+  <si>
+    <t>Anas platyrhynchos platyrhynchos</t>
+  </si>
+  <si>
+    <t>Dromaius novaehollandiae</t>
+  </si>
+  <si>
+    <t>Ficedula albicollis</t>
+  </si>
+  <si>
+    <t>Manacus vitellinus</t>
+  </si>
+  <si>
+    <t>Apteryx haastii</t>
+  </si>
+  <si>
+    <t>Parus major</t>
+  </si>
+  <si>
+    <t>Numida meleagris</t>
+  </si>
+  <si>
+    <t>Coturnix japonica</t>
+  </si>
+  <si>
+    <t>Apteryx owenii</t>
+  </si>
+  <si>
+    <t>Apteryx rowi</t>
+  </si>
+  <si>
+    <t>Chrysemys picta bellii</t>
+  </si>
+  <si>
+    <t>Anser brachyrhynchus</t>
+  </si>
+  <si>
+    <t>Calidris pugnax</t>
+  </si>
+  <si>
+    <t>Calidris pygmaea</t>
+  </si>
+  <si>
+    <t>Sphenodon punctatus</t>
+  </si>
+  <si>
+    <t>Meleagris gallopavo</t>
+  </si>
+  <si>
+    <t>Zonotrichia albicollis</t>
+  </si>
+  <si>
+    <t>Taeniopygia guttata</t>
+  </si>
+  <si>
+    <t>Testudines</t>
+  </si>
+  <si>
+    <t>Squamata</t>
+  </si>
+  <si>
+    <t>Crocodilia</t>
+  </si>
+  <si>
+    <t>Passeriformes</t>
+  </si>
+  <si>
+    <t>Psittaciformes</t>
+  </si>
+  <si>
+    <t>Tinamiformes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Anseriformes</t>
+  </si>
+  <si>
+    <t>Casuariiformes</t>
+  </si>
+  <si>
+    <t>Chicken</t>
+  </si>
+  <si>
+    <t>Gallus gallus</t>
+  </si>
+  <si>
+    <t>ggallus</t>
+  </si>
+  <si>
+    <t>Galliformes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Apterygiformes</t>
+  </si>
+  <si>
+    <t>Apterygiformes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Testudines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Charadriiformes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Rhynchocephalia</t>
+  </si>
+  <si>
+    <t>Ailuropoda melanoleuca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Colobus angolensis </t>
+  </si>
+  <si>
+    <t>Pongo abelii</t>
   </si>
 </sst>
 </file>
@@ -1283,24 +1614,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4CD8A07-9E83-CF4C-8D24-5A6C8326EE24}">
   <dimension ref="A1:D94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>184</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1311,10 +1648,10 @@
         <v>132</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>235</v>
+        <v>404</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1325,10 +1662,10 @@
         <v>106</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1339,10 +1676,10 @@
         <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1353,10 +1690,10 @@
         <v>182</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1367,10 +1704,10 @@
         <v>46</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1381,10 +1718,10 @@
         <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>186</v>
+        <v>405</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -1395,10 +1732,10 @@
         <v>26</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -1409,10 +1746,10 @@
         <v>160</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -1423,10 +1760,10 @@
         <v>6</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1437,10 +1774,10 @@
         <v>30</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -1451,10 +1788,10 @@
         <v>58</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -1465,10 +1802,10 @@
         <v>36</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -1479,10 +1816,10 @@
         <v>38</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -1493,10 +1830,10 @@
         <v>40</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1507,10 +1844,10 @@
         <v>74</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>211</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -1521,10 +1858,10 @@
         <v>158</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -1535,10 +1872,10 @@
         <v>110</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -1549,10 +1886,10 @@
         <v>104</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -1563,10 +1900,10 @@
         <v>56</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -1577,10 +1914,10 @@
         <v>84</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -1591,10 +1928,10 @@
         <v>178</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -1605,10 +1942,10 @@
         <v>166</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -1619,10 +1956,10 @@
         <v>18</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -1633,10 +1970,10 @@
         <v>94</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -1647,10 +1984,10 @@
         <v>62</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -1661,10 +1998,10 @@
         <v>88</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -1675,10 +2012,10 @@
         <v>86</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -1689,10 +2026,10 @@
         <v>102</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -1703,10 +2040,10 @@
         <v>32</v>
       </c>
       <c r="C30" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -1717,10 +2054,10 @@
         <v>50</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -1731,10 +2068,10 @@
         <v>80</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -1745,10 +2082,10 @@
         <v>120</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -1759,10 +2096,10 @@
         <v>122</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -1773,10 +2110,10 @@
         <v>90</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -1787,10 +2124,10 @@
         <v>162</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -1801,10 +2138,10 @@
         <v>100</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -1815,10 +2152,10 @@
         <v>66</v>
       </c>
       <c r="C38" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>207</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -1829,10 +2166,10 @@
         <v>76</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -1843,10 +2180,10 @@
         <v>150</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -1857,10 +2194,10 @@
         <v>128</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>232</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -1871,10 +2208,10 @@
         <v>48</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -1885,10 +2222,10 @@
         <v>64</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -1899,10 +2236,10 @@
         <v>114</v>
       </c>
       <c r="C44" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -1913,10 +2250,10 @@
         <v>4</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -1927,10 +2264,10 @@
         <v>108</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -1941,24 +2278,24 @@
         <v>118</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -1969,10 +2306,10 @@
         <v>136</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -1983,10 +2320,10 @@
         <v>142</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -1997,10 +2334,10 @@
         <v>156</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
@@ -2011,10 +2348,10 @@
         <v>68</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -2025,10 +2362,10 @@
         <v>164</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -2042,7 +2379,7 @@
         <v>185</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -2053,10 +2390,10 @@
         <v>116</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -2067,10 +2404,10 @@
         <v>180</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -2081,10 +2418,10 @@
         <v>176</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -2095,10 +2432,10 @@
         <v>72</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
@@ -2109,10 +2446,10 @@
         <v>12</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
@@ -2123,10 +2460,10 @@
         <v>152</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -2137,10 +2474,10 @@
         <v>144</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -2151,10 +2488,10 @@
         <v>54</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
@@ -2165,10 +2502,10 @@
         <v>28</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
@@ -2179,10 +2516,10 @@
         <v>138</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -2193,10 +2530,10 @@
         <v>130</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>234</v>
+        <v>406</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
@@ -2207,10 +2544,10 @@
         <v>126</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -2221,10 +2558,10 @@
         <v>92</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -2235,10 +2572,10 @@
         <v>96</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -2249,10 +2586,10 @@
         <v>44</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
@@ -2263,10 +2600,10 @@
         <v>124</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -2277,10 +2614,10 @@
         <v>24</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
@@ -2291,10 +2628,10 @@
         <v>98</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -2305,10 +2642,10 @@
         <v>82</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -2319,10 +2656,10 @@
         <v>170</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
@@ -2333,10 +2670,10 @@
         <v>174</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -2347,10 +2684,10 @@
         <v>34</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
@@ -2361,10 +2698,10 @@
         <v>112</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
@@ -2375,10 +2712,10 @@
         <v>20</v>
       </c>
       <c r="C78" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D78" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
@@ -2389,10 +2726,10 @@
         <v>146</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -2403,10 +2740,10 @@
         <v>78</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
@@ -2417,10 +2754,10 @@
         <v>154</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
@@ -2431,10 +2768,10 @@
         <v>22</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
@@ -2445,10 +2782,10 @@
         <v>52</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
@@ -2459,10 +2796,10 @@
         <v>168</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
@@ -2473,10 +2810,10 @@
         <v>134</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
@@ -2487,10 +2824,10 @@
         <v>172</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
@@ -2501,10 +2838,10 @@
         <v>70</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
@@ -2515,10 +2852,10 @@
         <v>60</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
@@ -2529,10 +2866,10 @@
         <v>10</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
@@ -2543,10 +2880,10 @@
         <v>140</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
@@ -2557,10 +2894,10 @@
         <v>16</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
@@ -2571,10 +2908,10 @@
         <v>2</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
@@ -2585,10 +2922,10 @@
         <v>42</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
@@ -2599,13 +2936,531 @@
         <v>148</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9714CDF1-10BC-6643-9617-A7E6A4D69335}">
+  <dimension ref="A1:E33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="E33" s="1"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B33">
+    <sortCondition ref="B2:B33"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>